<commit_message>
Fixed a visualization glitch in Synoptic Panel
</commit_message>
<xml_diff>
--- a/src/Clients/Visuals/visuals/sampledata/cardWithStates-Data.xlsx
+++ b/src/Clients/Visuals/visuals/sampledata/cardWithStates-Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Downloads\BackupVisuals\sampledata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\PowerBI-visuals\src\Clients\Visuals\visuals\sampledata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,12 +24,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Value</t>
   </si>
   <si>
     <t>State</t>
+  </si>
+  <si>
+    <t>Great to</t>
+  </si>
+  <si>
+    <t>Great from</t>
+  </si>
+  <si>
+    <t>Moderate from</t>
+  </si>
+  <si>
+    <t>Moderate to</t>
+  </si>
+  <si>
+    <t>Fail from</t>
+  </si>
+  <si>
+    <t>Fail to</t>
   </si>
 </sst>
 </file>
@@ -85,11 +103,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:B2" totalsRowShown="0">
-  <autoFilter ref="A1:B2"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H2" totalsRowShown="0">
+  <autoFilter ref="A1:H2"/>
+  <tableColumns count="8">
     <tableColumn id="1" name="Value"/>
-    <tableColumn id="2" name="State"/>
+    <tableColumn id="3" name="State"/>
+    <tableColumn id="8" name="Great from"/>
+    <tableColumn id="7" name="Great to"/>
+    <tableColumn id="6" name="Moderate from"/>
+    <tableColumn id="5" name="Moderate to"/>
+    <tableColumn id="4" name="Fail from"/>
+    <tableColumn id="2" name="Fail to"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -358,31 +382,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>369</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>40</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+      <c r="D2">
+        <v>1048576</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <v>50</v>
+      </c>
+      <c r="G2">
+        <v>-1048576</v>
+      </c>
+      <c r="H2">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>